<commit_message>
actualizacion de excel 2.requerimientos-funcionales
</commit_message>
<xml_diff>
--- a/analisis/documentos_cp/toma_documentos/2.requerimientos-funcionales.xlsx
+++ b/analisis/documentos_cp/toma_documentos/2.requerimientos-funcionales.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sala30401\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Clase_analisis\Proyecto_cpc\analisis\documentos_cp\toma_documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -140,12 +140,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -160,10 +172,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,16 +201,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -218,7 +234,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10220325" y="3190875"/>
+          <a:off x="6048375" y="0"/>
           <a:ext cx="5924550" cy="4267200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -504,250 +520,1386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C75"/>
+  <dimension ref="A2:AF76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C46" t="s">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C62" t="s">
+      <c r="B62" s="5"/>
+      <c r="C62" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
+      <c r="P62" s="5"/>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
+      <c r="P63" s="5"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="5"/>
+      <c r="P64" s="5"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5"/>
+      <c r="P65" s="5"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="5"/>
+      <c r="P66" s="5"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="5"/>
+      <c r="P67" s="5"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="5"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="5"/>
+      <c r="P68" s="5"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5"/>
+      <c r="L69" s="5"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="5"/>
+      <c r="O69" s="5"/>
+      <c r="P69" s="5"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="5"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="5"/>
+      <c r="P70" s="5"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="5"/>
+      <c r="M71" s="5"/>
+      <c r="N71" s="5"/>
+      <c r="O71" s="5"/>
+      <c r="P71" s="5"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
+      <c r="N72" s="5"/>
+      <c r="O72" s="5"/>
+      <c r="P72" s="5"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+      <c r="M73" s="5"/>
+      <c r="N73" s="5"/>
+      <c r="O73" s="5"/>
+      <c r="P73" s="5"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="5"/>
+      <c r="L74" s="5"/>
+      <c r="M74" s="5"/>
+      <c r="N74" s="5"/>
+      <c r="O74" s="5"/>
+      <c r="P74" s="5"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="5"/>
+      <c r="L75" s="5"/>
+      <c r="M75" s="5"/>
+      <c r="N75" s="5"/>
+      <c r="O75" s="5"/>
+      <c r="P75" s="5"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+      <c r="M76" s="5"/>
+      <c r="N76" s="5"/>
+      <c r="O76" s="5"/>
+      <c r="P76" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>